<commit_message>
Return to baseline with updated activities
AMAU=18, SSU=12, Hrs = 9-9, consultant = 1, Nurse = 3
Dist of activities = normal, 2 more activities for consultant (Approval
& Decision)
</commit_message>
<xml_diff>
--- a/Tallagh Model-baseline 1-11-2012/Model - Scenarios (laptop)/control.xlsx
+++ b/Tallagh Model-baseline 1-11-2012/Model - Scenarios (laptop)/control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5976" windowHeight="9324" tabRatio="843" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9384" tabRatio="843" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="34" state="hidden" r:id="rId1"/>
@@ -9829,9 +9829,7 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -16795,7 +16793,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17082,7 +17080,9 @@
   </sheetPr>
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -49284,8 +49284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49309,100 +49309,74 @@
   <sheetData>
     <row r="1" spans="2:16" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
-        <v>7.318548596294737</v>
+        <v>7.4290995365560804</v>
       </c>
       <c r="C1" s="68">
-        <v>13.625960786532396</v>
+        <v>13.912210254582837</v>
       </c>
       <c r="D1" s="68">
-        <v>5.6154092871583865</v>
+        <v>5.5595245735048717</v>
       </c>
       <c r="E1" s="68">
-        <v>9.497147970516048</v>
+        <v>9.2790035374952051</v>
       </c>
       <c r="F1" s="68">
-        <v>14.532446592272391</v>
+        <v>13.921257239105683</v>
       </c>
       <c r="G1" s="68">
-        <v>7.6840587636928488</v>
+        <v>7.4886092990853745</v>
       </c>
       <c r="H1" s="68">
-        <v>16.786169047877468</v>
+        <v>4.3209787010548917</v>
       </c>
       <c r="I1" s="68">
-        <v>16.761540137280459</v>
+        <v>4.9014125197762093</v>
       </c>
       <c r="J1" s="68">
-        <v>16.810240322762816</v>
+        <v>3.7410730295753551</v>
       </c>
       <c r="K1" s="84">
-        <v>2096</v>
+        <v>2197</v>
       </c>
       <c r="L1" s="84">
-        <v>12907</v>
+        <v>12920</v>
       </c>
       <c r="M1" s="84">
-        <v>415</v>
+        <v>391</v>
       </c>
       <c r="N1" s="192">
-        <v>77.676528338321845</v>
+        <v>64.483303105962506</v>
       </c>
       <c r="O1" s="159">
         <f>K1/L1</f>
-        <v>0.16239250019369333</v>
+        <v>0.17004643962848298</v>
       </c>
       <c r="P1" s="159">
         <f t="shared" ref="P1:P7" si="0">M1/K1</f>
-        <v>0.19799618320610687</v>
+        <v>0.17796995903504778</v>
       </c>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="68">
-        <v>5.7528149222556264</v>
-      </c>
-      <c r="C2" s="68">
-        <v>10.88960835828402</v>
-      </c>
-      <c r="D2" s="68">
-        <v>4.224854034182826</v>
-      </c>
-      <c r="E2" s="68">
-        <v>7.3243902626860695</v>
-      </c>
-      <c r="F2" s="68">
-        <v>11.643524002608586</v>
-      </c>
-      <c r="G2" s="68">
-        <v>5.6153179982196626</v>
-      </c>
-      <c r="H2" s="68">
-        <v>9.2549074853304703</v>
-      </c>
-      <c r="I2" s="68">
-        <v>9.4040788846585119</v>
-      </c>
-      <c r="J2" s="68">
-        <v>9.1669794757559249</v>
-      </c>
-      <c r="K2" s="84">
-        <v>3794</v>
-      </c>
-      <c r="L2" s="84">
-        <v>12837</v>
-      </c>
-      <c r="M2" s="84">
-        <v>804</v>
-      </c>
-      <c r="N2" s="192">
-        <v>71.8121525376188</v>
-      </c>
-      <c r="O2" s="159">
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="192"/>
+      <c r="O2" s="159" t="e">
         <f t="shared" ref="O2:O7" si="1">K2/L2</f>
-        <v>0.29555192023058346</v>
-      </c>
-      <c r="P2" s="159">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P2" s="159" t="e">
         <f t="shared" si="0"/>
-        <v>0.21191354770690565</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
@@ -49418,10 +49392,7 @@
       <c r="K3" s="84"/>
       <c r="L3" s="84"/>
       <c r="M3" s="84"/>
-      <c r="N3" s="192" t="e">
-        <f>K3/L3</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="N3" s="192"/>
       <c r="O3" s="159" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -49444,10 +49415,7 @@
       <c r="K4" s="84"/>
       <c r="L4" s="84"/>
       <c r="M4" s="84"/>
-      <c r="N4" s="192" t="e">
-        <f>K4/L4</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="N4" s="192"/>
       <c r="O4" s="159" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -49470,10 +49438,7 @@
       <c r="K5" s="84"/>
       <c r="L5" s="84"/>
       <c r="M5" s="84"/>
-      <c r="N5" s="192" t="e">
-        <f t="shared" ref="N5" si="2">K5/L5</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="N5" s="192"/>
       <c r="O5" s="159" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -49496,10 +49461,7 @@
       <c r="K6" s="84"/>
       <c r="L6" s="84"/>
       <c r="M6" s="84"/>
-      <c r="N6" s="192" t="e">
-        <f t="shared" ref="N6" si="3">K6/L6</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="N6" s="192"/>
       <c r="O6" s="159" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -49522,10 +49484,7 @@
       <c r="K7" s="84"/>
       <c r="L7" s="84"/>
       <c r="M7" s="84"/>
-      <c r="N7" s="192" t="e">
-        <f t="shared" ref="N7" si="4">K7/L7</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="N7" s="192"/>
       <c r="O7" s="159" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -49553,21 +49512,53 @@
       <c r="P8" s="159"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="68"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="84"/>
-      <c r="N9" s="192"/>
-      <c r="O9" s="159"/>
-      <c r="P9" s="159"/>
+      <c r="B9" s="68">
+        <v>7.1543488441325058</v>
+      </c>
+      <c r="C9" s="68">
+        <v>13.354340058327084</v>
+      </c>
+      <c r="D9" s="68">
+        <v>5.4497545554077211</v>
+      </c>
+      <c r="E9" s="68">
+        <v>8.9773243974963179</v>
+      </c>
+      <c r="F9" s="68">
+        <v>13.633949898521392</v>
+      </c>
+      <c r="G9" s="68">
+        <v>7.2265288328715735</v>
+      </c>
+      <c r="H9" s="68">
+        <v>9.3571601166914604</v>
+      </c>
+      <c r="I9" s="68">
+        <v>12.59335305097259</v>
+      </c>
+      <c r="J9" s="68">
+        <v>5.9567194839218383</v>
+      </c>
+      <c r="K9" s="84">
+        <v>2586</v>
+      </c>
+      <c r="L9" s="84">
+        <v>12790</v>
+      </c>
+      <c r="M9" s="84">
+        <v>491</v>
+      </c>
+      <c r="N9" s="192">
+        <v>90.915137034946497</v>
+      </c>
+      <c r="O9" s="159">
+        <f t="shared" ref="O9" si="2">K9/L9</f>
+        <v>0.20218921032056295</v>
+      </c>
+      <c r="P9" s="159">
+        <f t="shared" ref="P9" si="3">M9/K9</f>
+        <v>0.18986852281515854</v>
+      </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="68"/>
@@ -49612,60 +49603,60 @@
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="186">
-        <f t="shared" ref="B13:L13" si="5">AVERAGE(B1:B10)</f>
-        <v>6.5356817592751817</v>
+        <f t="shared" ref="B13:L13" si="4">AVERAGE(B1:B10)</f>
+        <v>7.2917241903442935</v>
       </c>
       <c r="C13" s="186">
-        <f t="shared" si="5"/>
-        <v>12.257784572408209</v>
+        <f t="shared" si="4"/>
+        <v>13.63327515645496</v>
       </c>
       <c r="D13" s="186">
-        <f t="shared" si="5"/>
-        <v>4.9201316606706058</v>
+        <f t="shared" si="4"/>
+        <v>5.504639564456296</v>
       </c>
       <c r="E13" s="186">
-        <f t="shared" si="5"/>
-        <v>8.4107691166010596</v>
+        <f t="shared" si="4"/>
+        <v>9.1281639674957624</v>
       </c>
       <c r="F13" s="186">
-        <f t="shared" si="5"/>
-        <v>13.08798529744049</v>
+        <f t="shared" si="4"/>
+        <v>13.777603568813538</v>
       </c>
       <c r="G13" s="186">
-        <f t="shared" si="5"/>
-        <v>6.6496883809562561</v>
+        <f t="shared" si="4"/>
+        <v>7.357569065978474</v>
       </c>
       <c r="H13" s="186">
-        <f t="shared" si="5"/>
-        <v>13.020538266603969</v>
+        <f t="shared" si="4"/>
+        <v>6.8390694088731756</v>
       </c>
       <c r="I13" s="186">
-        <f t="shared" si="5"/>
-        <v>13.082809510969486</v>
+        <f t="shared" si="4"/>
+        <v>8.7473827853744002</v>
       </c>
       <c r="J13" s="186">
-        <f t="shared" si="5"/>
-        <v>12.988609899259369</v>
+        <f t="shared" si="4"/>
+        <v>4.8488962567485965</v>
       </c>
       <c r="K13" s="186">
-        <f t="shared" si="5"/>
-        <v>2945</v>
+        <f t="shared" si="4"/>
+        <v>2391.5</v>
       </c>
       <c r="L13" s="186">
-        <f t="shared" si="5"/>
-        <v>12872</v>
+        <f t="shared" si="4"/>
+        <v>12855</v>
       </c>
       <c r="M13" s="186">
         <f>AVERAGE(M1:M10)</f>
-        <v>609.5</v>
-      </c>
-      <c r="N13" s="186" t="e">
+        <v>441</v>
+      </c>
+      <c r="N13" s="186">
         <f>AVERAGE(N1:N10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O13" s="187" t="e">
+        <v>77.699220070454501</v>
+      </c>
+      <c r="O13" s="187">
         <f>AVERAGE(N2:N10)</f>
-        <v>#DIV/0!</v>
+        <v>90.915137034946497</v>
       </c>
       <c r="P13" s="187" t="e">
         <f>AVERAGE(P2:P10)</f>
@@ -49754,51 +49745,51 @@
     <row r="17" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="76">
         <f>B13-B18</f>
-        <v>-1.6743182407248192</v>
+        <v>-0.91827580965570732</v>
       </c>
       <c r="C17" s="76">
-        <f t="shared" ref="C17:K17" si="6">C13-C18</f>
-        <v>-2.8822154275917917</v>
+        <f t="shared" ref="C17:K17" si="5">C13-C18</f>
+        <v>-1.5067248435450402</v>
       </c>
       <c r="D17" s="76">
+        <f t="shared" si="5"/>
+        <v>-0.3153604355437043</v>
+      </c>
+      <c r="E17" s="76">
+        <f t="shared" si="5"/>
+        <v>-1.2818360325042377</v>
+      </c>
+      <c r="F17" s="76">
+        <f t="shared" si="5"/>
+        <v>-2.5823964311864618</v>
+      </c>
+      <c r="G17" s="76">
+        <f t="shared" si="5"/>
+        <v>0.63756906597847429</v>
+      </c>
+      <c r="H17" s="76">
+        <f t="shared" si="5"/>
+        <v>2.3790694088731756</v>
+      </c>
+      <c r="I17" s="76">
+        <f t="shared" si="5"/>
+        <v>3.9273827853743999</v>
+      </c>
+      <c r="J17" s="76">
+        <f t="shared" si="5"/>
+        <v>0.75889625674859662</v>
+      </c>
+      <c r="K17" s="90">
+        <f t="shared" si="5"/>
+        <v>928.5</v>
+      </c>
+      <c r="L17" s="75"/>
+      <c r="O17" s="76">
+        <f t="shared" ref="O17:P17" si="6">O13-O18</f>
+        <v>90.7551370349465</v>
+      </c>
+      <c r="P17" s="76" t="e">
         <f t="shared" si="6"/>
-        <v>-0.89986833932939447</v>
-      </c>
-      <c r="E17" s="76">
-        <f t="shared" si="6"/>
-        <v>-1.9992308833989405</v>
-      </c>
-      <c r="F17" s="76">
-        <f t="shared" si="6"/>
-        <v>-3.2720147025595097</v>
-      </c>
-      <c r="G17" s="76">
-        <f t="shared" si="6"/>
-        <v>-7.0311619043743612E-2</v>
-      </c>
-      <c r="H17" s="76">
-        <f t="shared" si="6"/>
-        <v>8.5605382666039702</v>
-      </c>
-      <c r="I17" s="76">
-        <f t="shared" si="6"/>
-        <v>8.2628095109694861</v>
-      </c>
-      <c r="J17" s="76">
-        <f t="shared" si="6"/>
-        <v>8.8986098992593696</v>
-      </c>
-      <c r="K17" s="90">
-        <f t="shared" si="6"/>
-        <v>1482</v>
-      </c>
-      <c r="L17" s="75"/>
-      <c r="O17" s="76" t="e">
-        <f t="shared" ref="O17:P17" si="7">O13-O18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P17" s="76" t="e">
-        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -49835,7 +49826,7 @@
       </c>
       <c r="M18" s="74">
         <f>M13/K13</f>
-        <v>0.20696095076400678</v>
+        <v>0.18440309429228519</v>
       </c>
       <c r="O18" s="74">
         <v>0.16</v>
@@ -49846,51 +49837,51 @@
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="73">
-        <f t="shared" ref="B19:D19" si="8">B17/B18</f>
-        <v>-0.20393644832214605</v>
+        <f t="shared" ref="B19:D19" si="7">B17/B18</f>
+        <v>-0.11184845428205935</v>
       </c>
       <c r="C19" s="73">
-        <f t="shared" si="8"/>
-        <v>-0.19037090010513816</v>
+        <f t="shared" si="7"/>
+        <v>-9.9519474474573322E-2</v>
       </c>
       <c r="D19" s="73">
-        <f t="shared" si="8"/>
-        <v>-0.1546165531493805</v>
+        <f t="shared" si="7"/>
+        <v>-5.41856418459973E-2</v>
       </c>
       <c r="E19" s="73">
         <f>E17/E18</f>
-        <v>-0.19204907621507594</v>
+        <v>-0.12313506556236674</v>
       </c>
       <c r="F19" s="73">
-        <f t="shared" ref="F19:K19" si="9">F17/F18</f>
-        <v>-0.20000089868945659</v>
+        <f t="shared" ref="F19:K19" si="8">F17/F18</f>
+        <v>-0.15784819261530941</v>
       </c>
       <c r="G19" s="73">
+        <f t="shared" si="8"/>
+        <v>9.4876349103939633E-2</v>
+      </c>
+      <c r="H19" s="73">
+        <f t="shared" si="8"/>
+        <v>0.53342363427649675</v>
+      </c>
+      <c r="I19" s="73">
+        <f t="shared" si="8"/>
+        <v>0.81480970650921158</v>
+      </c>
+      <c r="J19" s="73">
+        <f t="shared" si="8"/>
+        <v>0.18554920702899674</v>
+      </c>
+      <c r="K19" s="73">
+        <f t="shared" si="8"/>
+        <v>0.63465481886534514</v>
+      </c>
+      <c r="O19" s="73">
+        <f t="shared" ref="O19:P19" si="9">O17/O18</f>
+        <v>567.21960646841558</v>
+      </c>
+      <c r="P19" s="73" t="e">
         <f t="shared" si="9"/>
-        <v>-1.0463038548176134E-2</v>
-      </c>
-      <c r="H19" s="73">
-        <f t="shared" si="9"/>
-        <v>1.9194031987901279</v>
-      </c>
-      <c r="I19" s="73">
-        <f t="shared" si="9"/>
-        <v>1.7142758321513456</v>
-      </c>
-      <c r="J19" s="73">
-        <f t="shared" si="9"/>
-        <v>2.1756992418727066</v>
-      </c>
-      <c r="K19" s="73">
-        <f t="shared" si="9"/>
-        <v>1.0129870129870129</v>
-      </c>
-      <c r="O19" s="73" t="e">
-        <f t="shared" ref="O19:P19" si="10">O17/O18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P19" s="73" t="e">
-        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -49920,66 +49911,66 @@
   <sheetData>
     <row r="1" spans="2:11" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68">
-        <v>8.5469780578722254</v>
+        <v>8.5817210911332928</v>
       </c>
       <c r="C1" s="68">
-        <v>14.793453717827486</v>
+        <v>15.026918935278815</v>
       </c>
       <c r="D1" s="68">
-        <v>6.8602929453154315</v>
+        <v>6.7230792993433282</v>
       </c>
       <c r="E1" s="68">
-        <v>46.664370191755658</v>
+        <v>46.781411359724615</v>
       </c>
       <c r="F1" s="68">
-        <v>56.934557979334102</v>
+        <v>57.767324460761813</v>
       </c>
       <c r="G1" s="68">
-        <v>58.00524934383202</v>
+        <v>59.083518107908347</v>
       </c>
       <c r="H1" s="68">
-        <v>67.181804927832047</v>
+        <v>69.287614543304755</v>
       </c>
       <c r="I1" s="68">
-        <v>0.88673497646081423</v>
+        <v>0.90886858619416755</v>
       </c>
       <c r="J1" s="68">
-        <v>0.24669989845841411</v>
+        <v>0.26047434477667036</v>
       </c>
       <c r="K1" s="68">
-        <v>9.0602787778085475E-2</v>
+        <v>6.9905869324473971E-2</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="68">
-        <v>6.9293265793787384</v>
+        <v>8.3063571667846006</v>
       </c>
       <c r="C2" s="68">
-        <v>12.037196976688206</v>
+        <v>14.457679296893254</v>
       </c>
       <c r="D2" s="68">
-        <v>5.4099689712464674</v>
+        <v>6.6151437103713819</v>
       </c>
       <c r="E2" s="68">
-        <v>58.316127552190864</v>
+        <v>48.611583361668366</v>
       </c>
       <c r="F2" s="68">
-        <v>71.384333065718536</v>
+        <v>60.176790571169533</v>
       </c>
       <c r="G2" s="68">
-        <v>72.767857142857139</v>
+        <v>60.814911140008668</v>
       </c>
       <c r="H2" s="68">
-        <v>81.431334622823982</v>
+        <v>71.453337185784463</v>
       </c>
       <c r="I2" s="68">
-        <v>0.89088634573506931</v>
+        <v>0.9060160798447463</v>
       </c>
       <c r="J2" s="68">
-        <v>0.24005003938284761</v>
+        <v>0.25561408372608818</v>
       </c>
       <c r="K2" s="68">
-        <v>7.0379465319927725E-2</v>
+        <v>6.9540707882820435E-2</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
@@ -50205,43 +50196,43 @@
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="67">
         <f>AVERAGE(B1:B10)</f>
-        <v>7.8046043886277658</v>
+        <v>8.006286334437327</v>
       </c>
       <c r="C13" s="67">
         <f t="shared" ref="C13:J13" si="0">AVERAGE(C1:C10)</f>
-        <v>13.486465300743337</v>
+        <v>13.865600663265676</v>
       </c>
       <c r="D13" s="67">
         <f t="shared" si="0"/>
-        <v>6.1996496774575531</v>
+        <v>6.3522155479079538</v>
       </c>
       <c r="E13" s="67">
         <f t="shared" si="0"/>
-        <v>51.71330819398657</v>
+        <v>50.343664905050346</v>
       </c>
       <c r="F13" s="67">
         <f t="shared" si="0"/>
-        <v>63.940423155950121</v>
+        <v>62.458312296932796</v>
       </c>
       <c r="G13" s="67">
         <f t="shared" si="0"/>
-        <v>64.51653533859276</v>
+        <v>62.963010018768173</v>
       </c>
       <c r="H13" s="67">
         <f t="shared" si="0"/>
-        <v>74.220779442657516</v>
+        <v>73.096181182433682</v>
       </c>
       <c r="I13" s="67">
         <f t="shared" si="0"/>
-        <v>0.90839362424975179</v>
+        <v>0.91371695908447059</v>
       </c>
       <c r="J13" s="67">
         <f t="shared" si="0"/>
-        <v>0.2541833270095914</v>
+        <v>0.25837453996123372</v>
       </c>
       <c r="K13" s="67">
         <f>AVERAGE(K1:K10)</f>
-        <v>6.1522187733659819E-2</v>
+        <v>5.8445662606414275E-2</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -50363,8 +50354,8 @@
   </sheetPr>
   <dimension ref="A1:AY19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1:AF2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -50376,16 +50367,20 @@
     <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" hidden="1" customWidth="1"/>
+    <col min="12" max="13" width="9" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9.21875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="0" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="10.109375" hidden="1" customWidth="1"/>
+    <col min="22" max="23" width="9" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="0" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="10.109375" bestFit="1" customWidth="1"/>
@@ -50451,43 +50446,43 @@
         <v>103</v>
       </c>
       <c r="Z1" s="167">
-        <v>22459.369148532081</v>
+        <v>14472.951480567162</v>
       </c>
       <c r="AA1" s="167">
-        <v>26405.003439548949</v>
+        <v>22606.634951736305</v>
       </c>
       <c r="AB1" s="167">
-        <v>11639.359033707809</v>
+        <v>9572.6787571040913</v>
       </c>
       <c r="AC1" s="167">
-        <v>15418.33047602413</v>
+        <v>15844.888519323036</v>
       </c>
       <c r="AD1" s="167">
-        <v>37193.426007694587</v>
+        <v>24777.495151911797</v>
       </c>
       <c r="AE1" s="167">
-        <v>82037.546189104207</v>
+        <v>17012.954676921509</v>
       </c>
       <c r="AF1" s="167">
-        <v>99676.696138241197</v>
+        <v>51514.520058104608</v>
       </c>
       <c r="AG1" s="167">
-        <v>85524.88147097308</v>
+        <v>46910.282310058799</v>
       </c>
       <c r="AH1" s="167">
         <v>0</v>
       </c>
       <c r="AI1" s="167">
-        <v>51474.596540509403</v>
+        <v>18156.380496702055</v>
       </c>
       <c r="AJ1" s="167">
-        <v>22388.970517963327</v>
+        <v>16635.551611852447</v>
       </c>
       <c r="AK1" s="167">
-        <v>17353.376336803733</v>
+        <v>19248.650784593519</v>
       </c>
       <c r="AL1" s="185">
-        <v>2096</v>
+        <v>2197</v>
       </c>
       <c r="AO1" s="156" t="s">
         <v>263</v>
@@ -50520,111 +50515,72 @@
         <v>64</v>
       </c>
       <c r="B2" s="38">
-        <v>0.16666277685718911</v>
+        <v>0.16666278247764607</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="36">
-        <v>0.28899765373610636</v>
+        <v>0.29574374063844855</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>80</v>
       </c>
       <c r="F2" s="37">
-        <v>512.81868347233353</v>
+        <v>514.90326546799758</v>
       </c>
       <c r="G2">
         <f>F2/1440</f>
-        <v>0.35612408574467608</v>
+        <v>0.35757171213055389</v>
       </c>
       <c r="J2" s="169" t="s">
         <v>254</v>
       </c>
       <c r="K2" s="167">
-        <v>1977.1741813059366</v>
+        <v>1908.1325514390669</v>
       </c>
       <c r="L2" s="167">
         <f>K2/60</f>
-        <v>32.952903021765607</v>
+        <v>31.802209190651116</v>
       </c>
       <c r="M2" s="167">
         <f>L2/24</f>
-        <v>1.3730376259069004</v>
+        <v>1.3250920496104632</v>
       </c>
       <c r="N2" s="167"/>
       <c r="O2" s="168" t="s">
         <v>254</v>
       </c>
       <c r="P2" s="167">
-        <v>74363.514621700364</v>
+        <v>75890.106841206609</v>
       </c>
       <c r="Q2" s="167">
         <f>P2/60</f>
-        <v>1239.3919103616727</v>
+        <v>1264.83511402011</v>
       </c>
       <c r="R2" s="167">
         <f>Q2/24</f>
-        <v>51.641329598403026</v>
+        <v>52.701463084171252</v>
       </c>
       <c r="S2" s="167"/>
       <c r="T2" s="168" t="s">
         <v>254</v>
       </c>
       <c r="U2" s="167">
-        <v>48919.803360076192</v>
+        <v>49138.480067727731</v>
       </c>
       <c r="V2" s="167">
         <f>U2/60</f>
-        <v>815.3300560012699</v>
+        <v>818.97466779546221</v>
       </c>
       <c r="W2" s="167">
         <f>V2/24</f>
-        <v>33.972085666719579</v>
+        <v>34.123944491477594</v>
       </c>
       <c r="X2" s="156"/>
       <c r="Y2" s="184">
         <v>2</v>
       </c>
-      <c r="Z2" s="167">
-        <v>22437.321870195017</v>
-      </c>
-      <c r="AA2" s="167">
-        <v>43258.456901449659</v>
-      </c>
-      <c r="AB2" s="167">
-        <v>13796.004567839755</v>
-      </c>
-      <c r="AC2" s="167">
-        <v>20652.980579368796</v>
-      </c>
-      <c r="AD2" s="167">
-        <v>45025.546373099729</v>
-      </c>
-      <c r="AE2" s="167">
-        <v>91909.004323896836</v>
-      </c>
-      <c r="AF2" s="167">
-        <v>52526.400192726833</v>
-      </c>
-      <c r="AG2" s="167">
-        <v>118386.8728066575</v>
-      </c>
-      <c r="AH2" s="167">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="167">
-        <v>44100.558163853697</v>
-      </c>
-      <c r="AJ2" s="167">
-        <v>27165.820616259429</v>
-      </c>
-      <c r="AK2" s="167">
-        <v>16466.975994039858</v>
-      </c>
-      <c r="AL2" s="185">
-        <v>3794</v>
-      </c>
       <c r="AN2" s="175" t="s">
         <v>4</v>
       </c>
@@ -50663,7 +50619,7 @@
         <v>267</v>
       </c>
       <c r="AY2" s="183">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.3">
@@ -50677,57 +50633,57 @@
         <v>2</v>
       </c>
       <c r="D3" s="36">
-        <v>0.29247010037106325</v>
+        <v>0.29864270645105434</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>73</v>
       </c>
       <c r="F3" s="37">
-        <v>46.642947320096404</v>
+        <v>46.759949535497192</v>
       </c>
       <c r="J3" s="169" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="167">
-        <v>29926.780628803215</v>
+        <v>29942.776414506705</v>
       </c>
       <c r="L3" s="167">
         <f>K3/60</f>
-        <v>498.77967714672025</v>
+        <v>499.04627357511174</v>
       </c>
       <c r="M3" s="167">
         <f>L3/24</f>
-        <v>20.78248654778001</v>
+        <v>20.793594732296324</v>
       </c>
       <c r="N3" s="167"/>
       <c r="O3" s="168" t="s">
         <v>79</v>
       </c>
       <c r="P3" s="167">
-        <v>245016.13165681515</v>
+        <v>251573.13751412791</v>
       </c>
       <c r="Q3" s="167">
         <f>P3/60</f>
-        <v>4083.6021942802527</v>
+        <v>4192.8856252354653</v>
       </c>
       <c r="R3" s="167">
         <f>Q3/24</f>
-        <v>170.15009142834387</v>
+        <v>174.7035677181444</v>
       </c>
       <c r="S3" s="167"/>
       <c r="T3" s="168" t="s">
         <v>79</v>
       </c>
       <c r="U3" s="167">
-        <v>153757.62044133557</v>
+        <v>151872.58204802225</v>
       </c>
       <c r="V3" s="167">
         <f>U3/60</f>
-        <v>2562.6270073555929</v>
+        <v>2531.2097008003707</v>
       </c>
       <c r="W3" s="167">
         <f>V3/24</f>
-        <v>106.77612530648304</v>
+        <v>105.46707086668211</v>
       </c>
       <c r="X3" s="156"/>
       <c r="Y3" s="184">
@@ -50786,63 +50742,63 @@
         <v>83</v>
       </c>
       <c r="B4" s="38">
-        <v>18.481375358166186</v>
+        <v>19.876453488372086</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="36">
-        <v>7.228403394551719E-2</v>
+        <v>7.1261966518101155E-2</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>74</v>
       </c>
       <c r="F4" s="37">
-        <v>56.908423226991047</v>
+        <v>57.740825688073393</v>
       </c>
       <c r="J4" s="169" t="s">
         <v>15</v>
       </c>
       <c r="K4" s="167">
-        <v>1578.748450698964</v>
+        <v>1416.0413029557349</v>
       </c>
       <c r="L4" s="167">
         <f t="shared" ref="L4:L14" si="0">K4/60</f>
-        <v>26.312474178316066</v>
+        <v>23.600688382595582</v>
       </c>
       <c r="M4" s="167">
         <f t="shared" ref="M4:M14" si="1">L4/24</f>
-        <v>1.0963530907631693</v>
+        <v>0.98336201594148254</v>
       </c>
       <c r="N4" s="167"/>
       <c r="O4" s="168" t="s">
         <v>111</v>
       </c>
       <c r="P4" s="167">
-        <v>96494.633645765905</v>
+        <v>97617.405061876882</v>
       </c>
       <c r="Q4" s="167">
         <f t="shared" ref="Q4:Q14" si="2">P4/60</f>
-        <v>1608.2438940960985</v>
+        <v>1626.9567510312813</v>
       </c>
       <c r="R4" s="167">
         <f t="shared" ref="R4:R14" si="3">Q4/24</f>
-        <v>67.010162254004101</v>
+        <v>67.789864626303384</v>
       </c>
       <c r="S4" s="167"/>
       <c r="T4" s="168" t="s">
         <v>17</v>
       </c>
       <c r="U4" s="167">
-        <v>3639.799975351928</v>
+        <v>3499.844418734157</v>
       </c>
       <c r="V4" s="167">
         <f t="shared" ref="V4:V13" si="4">U4/60</f>
-        <v>60.663332922532135</v>
+        <v>58.330740312235953</v>
       </c>
       <c r="W4" s="167">
         <f t="shared" ref="W4:W13" si="5">V4/24</f>
-        <v>2.5276388717721723</v>
+        <v>2.4304475130098315</v>
       </c>
       <c r="X4" s="156"/>
       <c r="Y4" s="184">
@@ -50901,63 +50857,63 @@
         <v>84</v>
       </c>
       <c r="B5" s="38">
-        <v>80.169705870354463</v>
+        <v>81.110184854379199</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>70</v>
       </c>
       <c r="D5" s="36">
-        <v>62.239687525282939</v>
+        <v>63.875555163678627</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>75</v>
       </c>
       <c r="F5" s="37">
-        <v>7.4638015575425465</v>
+        <v>7.4379447765442768</v>
       </c>
       <c r="J5" s="169" t="s">
         <v>111</v>
       </c>
       <c r="K5" s="167">
-        <v>4164.3259169834973</v>
+        <v>4108.9171549239618</v>
       </c>
       <c r="L5" s="167">
         <f t="shared" si="0"/>
-        <v>69.405431949724957</v>
+        <v>68.481952582066029</v>
       </c>
       <c r="M5" s="167">
         <f t="shared" si="1"/>
-        <v>2.8918929979052064</v>
+        <v>2.853414690919418</v>
       </c>
       <c r="N5" s="167"/>
       <c r="O5" s="168" t="s">
         <v>112</v>
       </c>
       <c r="P5" s="167">
-        <v>141849.6573238596</v>
+        <v>144540.0778769257</v>
       </c>
       <c r="Q5" s="167">
         <f t="shared" si="2"/>
-        <v>2364.16095539766</v>
+        <v>2409.0012979487615</v>
       </c>
       <c r="R5" s="167">
         <f t="shared" si="3"/>
-        <v>98.506706474902501</v>
+        <v>100.3750540811984</v>
       </c>
       <c r="S5" s="167"/>
       <c r="T5" s="168" t="s">
         <v>111</v>
       </c>
       <c r="U5" s="167">
-        <v>141497.99664044369</v>
+        <v>137996.61834764987</v>
       </c>
       <c r="V5" s="167">
         <f t="shared" si="4"/>
-        <v>2358.299944007395</v>
+        <v>2299.943639127498</v>
       </c>
       <c r="W5" s="167">
         <f t="shared" si="5"/>
-        <v>98.262497666974795</v>
+        <v>95.830984963645747</v>
       </c>
       <c r="X5" s="156"/>
       <c r="Y5" s="184">
@@ -50982,37 +50938,37 @@
         <v>85</v>
       </c>
       <c r="B6" s="38">
-        <v>32.574033868866778</v>
+        <v>32.153994393833287</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>71</v>
       </c>
       <c r="D6" s="36">
-        <v>0.17871527169437937</v>
+        <v>0.17937457394675033</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>76</v>
       </c>
       <c r="F6" s="37">
-        <v>436.83125908593325</v>
+        <v>283.35386355455478</v>
       </c>
       <c r="G6">
         <f>F6/1440</f>
-        <v>0.30335504103189809</v>
+        <v>0.1967735163573297</v>
       </c>
       <c r="J6" s="169" t="s">
         <v>112</v>
       </c>
       <c r="K6" s="167">
-        <v>7317.3042510483529</v>
+        <v>7262.5465877209272</v>
       </c>
       <c r="L6" s="167">
         <f t="shared" si="0"/>
-        <v>121.95507085080588</v>
+        <v>121.04244312868212</v>
       </c>
       <c r="M6" s="167">
         <f t="shared" si="1"/>
-        <v>5.0814612854502448</v>
+        <v>5.0434351303617548</v>
       </c>
       <c r="N6" s="167"/>
       <c r="O6" s="172" t="s">
@@ -51028,15 +50984,15 @@
         <v>112</v>
       </c>
       <c r="U6" s="167">
-        <v>26122.972747605592</v>
+        <v>26473.200008212665</v>
       </c>
       <c r="V6" s="167">
         <f t="shared" ref="V6" si="6">U6/60</f>
-        <v>435.38287912675986</v>
+        <v>441.22000013687773</v>
       </c>
       <c r="W6" s="167">
         <f t="shared" ref="W6" si="7">V6/24</f>
-        <v>18.140953296948329</v>
+        <v>18.384166672369904</v>
       </c>
       <c r="X6" s="156"/>
       <c r="Y6" s="184">
@@ -51090,13 +51046,13 @@
         <v>103</v>
       </c>
       <c r="B7" s="38">
-        <v>138.55741449976497</v>
+        <v>34.958728714415614</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="36">
-        <v>0.52246471153598051</v>
+        <v>0.5220112581079025</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>77</v>
@@ -51170,15 +51126,15 @@
       </c>
       <c r="AQ7" s="176">
         <f>AQ2*$AG$11</f>
-        <v>101955.8771388153</v>
+        <v>64760.587693955531</v>
       </c>
       <c r="AR7" s="176">
         <f>AR2*$AI$11</f>
-        <v>47787.57735218155</v>
+        <v>25534.844668734848</v>
       </c>
       <c r="AS7" s="176">
         <f>AS2*$AB$11</f>
-        <v>12717.681800773782</v>
+        <v>10513.442555499609</v>
       </c>
       <c r="AT7" s="176">
         <f>AT2*$AJ$11</f>
@@ -51195,11 +51151,11 @@
       <c r="AW7" s="156"/>
       <c r="AX7" s="181">
         <f>SUM(AO7:AU7)+AE11+AF11</f>
-        <v>325535.95971375518</v>
+        <v>182164.77506029891</v>
       </c>
       <c r="AY7" s="179">
         <f>AX7/(1*$AY$2*60*125)</f>
-        <v>2.5532232134412172</v>
+        <v>1.7349026196218944</v>
       </c>
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.3">
@@ -51207,17 +51163,17 @@
         <v>7</v>
       </c>
       <c r="D8" s="36">
-        <v>8.22131670559553E-2</v>
+        <v>8.3727659668181964E-2</v>
       </c>
       <c r="E8" s="35" t="s">
         <v>78</v>
       </c>
       <c r="F8" s="37">
-        <v>8.7771583979080461</v>
+        <v>0.68185500519292774</v>
       </c>
       <c r="G8">
         <f>F8/1440</f>
-        <v>6.095248887436143E-3</v>
+        <v>4.7351042027286649E-4</v>
       </c>
       <c r="J8" s="173" t="s">
         <v>261</v>
@@ -51277,7 +51233,7 @@
       </c>
       <c r="AP8" s="176">
         <f>AP3*$AA$11</f>
-        <v>34831.730170499301</v>
+        <v>25269.392645293046</v>
       </c>
       <c r="AQ8" s="176">
         <f t="shared" ref="AQ8:AQ9" si="12">AQ3*$AG$11</f>
@@ -51285,11 +51241,11 @@
       </c>
       <c r="AR8" s="176">
         <f>AR3*$AI$11</f>
-        <v>47787.57735218155</v>
+        <v>25534.844668734848</v>
       </c>
       <c r="AS8" s="176">
         <f>AS3*$AB$11</f>
-        <v>12717.681800773782</v>
+        <v>10513.442555499609</v>
       </c>
       <c r="AT8" s="176">
         <f>AT3*$AJ$11</f>
@@ -51306,11 +51262,11 @@
       <c r="AW8" s="180"/>
       <c r="AX8" s="181">
         <f>SUM(AO8:AU8)+AF11</f>
-        <v>171438.53748893863</v>
+        <v>121706.11288177322</v>
       </c>
       <c r="AY8" s="178">
         <f>AX8/(2*$AY$2*60*125)</f>
-        <v>0.67230799015270049</v>
+        <v>0.57955291848463442</v>
       </c>
     </row>
     <row r="9" spans="1:51" x14ac:dyDescent="0.3">
@@ -51356,62 +51312,88 @@
       <c r="Y9" s="184">
         <v>9</v>
       </c>
-      <c r="Z9" s="167"/>
-      <c r="AA9" s="167"/>
-      <c r="AB9" s="167"/>
-      <c r="AC9" s="167"/>
-      <c r="AD9" s="167"/>
-      <c r="AE9" s="167"/>
-      <c r="AF9" s="167"/>
-      <c r="AG9" s="167"/>
-      <c r="AH9" s="167"/>
-      <c r="AI9" s="167"/>
-      <c r="AJ9" s="167"/>
-      <c r="AK9" s="167"/>
-      <c r="AL9" s="185"/>
+      <c r="Z9" s="167">
+        <v>22477.371681435907</v>
+      </c>
+      <c r="AA9" s="167">
+        <v>27932.150338849791</v>
+      </c>
+      <c r="AB9" s="167">
+        <v>11454.206353895128</v>
+      </c>
+      <c r="AC9" s="167">
+        <v>18178.958606963773</v>
+      </c>
+      <c r="AD9" s="167">
+        <v>38871.220311945362</v>
+      </c>
+      <c r="AE9" s="167">
+        <v>24921.979582804917</v>
+      </c>
+      <c r="AF9" s="167">
+        <v>69262.345966386827</v>
+      </c>
+      <c r="AG9" s="167">
+        <v>82610.893077852263</v>
+      </c>
+      <c r="AH9" s="167">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="167">
+        <v>32913.308840767641</v>
+      </c>
+      <c r="AJ9" s="167">
+        <v>50091.107807221517</v>
+      </c>
+      <c r="AK9" s="167">
+        <v>148563.29089924216</v>
+      </c>
+      <c r="AL9" s="185">
+        <v>2586</v>
+      </c>
       <c r="AN9" s="175" t="s">
         <v>5</v>
       </c>
       <c r="AO9" s="176">
         <f>AO4*$Z$11</f>
-        <v>22448.345509363549</v>
+        <v>18475.161581001536</v>
       </c>
       <c r="AP9" s="176">
         <f>AP4*$AA$11</f>
-        <v>34831.730170499301</v>
+        <v>25269.392645293046</v>
       </c>
       <c r="AQ9" s="176">
         <f t="shared" si="12"/>
-        <v>101955.8771388153</v>
+        <v>64760.587693955531</v>
       </c>
       <c r="AR9" s="176">
         <f>AR4*$AI$11</f>
-        <v>47787.57735218155</v>
+        <v>25534.844668734848</v>
       </c>
       <c r="AS9" s="176">
         <f>AS4*$AB$11</f>
-        <v>12717.681800773782</v>
+        <v>10513.442555499609</v>
       </c>
       <c r="AT9" s="176">
         <f>AT4*$AJ$11</f>
-        <v>24777.39556711138</v>
+        <v>33363.329709536978</v>
       </c>
       <c r="AU9" s="176">
         <f>AU4*$AK$11</f>
-        <v>16910.176165421795</v>
+        <v>83905.970841917835</v>
       </c>
       <c r="AV9" s="176">
         <f>($AC$11+$AD$11)*AV4</f>
-        <v>59145.141718093626</v>
+        <v>48836.281295071982</v>
       </c>
       <c r="AW9" s="180"/>
       <c r="AX9" s="177">
         <f>SUM(AO9:AV9)</f>
-        <v>320573.92542226025</v>
+        <v>310659.0109910114</v>
       </c>
       <c r="AY9" s="178">
         <f>AX9/(3*$AY$2*60*125)</f>
-        <v>0.83810176580983076</v>
+        <v>0.98621908251114732</v>
       </c>
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.3">
@@ -51428,15 +51410,15 @@
         <v>16</v>
       </c>
       <c r="P10" s="167">
-        <v>85658.662873684487</v>
+        <v>87349.34216803161</v>
       </c>
       <c r="Q10" s="167">
         <f t="shared" si="2"/>
-        <v>1427.6443812280747</v>
+        <v>1455.8223694671935</v>
       </c>
       <c r="R10" s="167">
         <f t="shared" si="3"/>
-        <v>59.485182551169778</v>
+        <v>60.659265394466395</v>
       </c>
       <c r="S10" s="167"/>
       <c r="T10" s="172" t="s">
@@ -51471,15 +51453,15 @@
         <v>16</v>
       </c>
       <c r="K11" s="167">
-        <v>2355.5282888140277</v>
+        <v>2222.4206490866632</v>
       </c>
       <c r="L11" s="167">
         <f t="shared" si="0"/>
-        <v>39.258804813567131</v>
+        <v>37.040344151444387</v>
       </c>
       <c r="M11" s="167">
         <f t="shared" si="1"/>
-        <v>1.6357835338986304</v>
+        <v>1.5433476729768494</v>
       </c>
       <c r="N11" s="167"/>
       <c r="O11" s="172" t="s">
@@ -51501,49 +51483,49 @@
         <v>16</v>
       </c>
       <c r="U11" s="167">
-        <v>29952.646009238364</v>
+        <v>29325.763442954256</v>
       </c>
       <c r="V11" s="167">
         <f t="shared" si="4"/>
-        <v>499.21076682063938</v>
+        <v>488.76272404923759</v>
       </c>
       <c r="W11" s="167">
         <f t="shared" si="5"/>
-        <v>20.800448617526641</v>
+        <v>20.365113502051567</v>
       </c>
       <c r="X11" s="156"/>
       <c r="Y11" s="168"/>
       <c r="Z11" s="167">
         <f>AVERAGE(Z1:Z10)</f>
-        <v>22448.345509363549</v>
+        <v>18475.161581001536</v>
       </c>
       <c r="AA11" s="167">
         <f t="shared" ref="AA11:AL11" si="13">AVERAGE(AA1:AA10)</f>
-        <v>34831.730170499301</v>
+        <v>25269.392645293046</v>
       </c>
       <c r="AB11" s="167">
         <f t="shared" si="13"/>
-        <v>12717.681800773782</v>
+        <v>10513.442555499609</v>
       </c>
       <c r="AC11" s="167">
         <f t="shared" si="13"/>
-        <v>18035.655527696465</v>
+        <v>17011.923563143406</v>
       </c>
       <c r="AD11" s="167">
         <f t="shared" si="13"/>
-        <v>41109.486190397161</v>
+        <v>31824.35773192858</v>
       </c>
       <c r="AE11" s="167">
         <f t="shared" si="13"/>
-        <v>86973.275256500521</v>
+        <v>20967.467129863213</v>
       </c>
       <c r="AF11" s="167">
         <f t="shared" si="13"/>
-        <v>76101.548165484011</v>
+        <v>60388.433012245718</v>
       </c>
       <c r="AG11" s="167">
         <f t="shared" si="13"/>
-        <v>101955.8771388153</v>
+        <v>64760.587693955531</v>
       </c>
       <c r="AH11" s="167">
         <f t="shared" si="13"/>
@@ -51551,19 +51533,19 @@
       </c>
       <c r="AI11" s="167">
         <f t="shared" si="13"/>
-        <v>47787.57735218155</v>
+        <v>25534.844668734848</v>
       </c>
       <c r="AJ11" s="167">
         <f t="shared" si="13"/>
-        <v>24777.39556711138</v>
+        <v>33363.329709536978</v>
       </c>
       <c r="AK11" s="167">
         <f t="shared" si="13"/>
-        <v>16910.176165421795</v>
+        <v>83905.970841917835</v>
       </c>
       <c r="AL11" s="185">
         <f t="shared" si="13"/>
-        <v>2945</v>
+        <v>2391.5</v>
       </c>
     </row>
     <row r="12" spans="1:51" x14ac:dyDescent="0.3">
@@ -51575,45 +51557,45 @@
         <v>17</v>
       </c>
       <c r="K12" s="167">
-        <v>3041.1456681152304</v>
+        <v>2955.6581735760792</v>
       </c>
       <c r="L12" s="167">
         <f t="shared" si="0"/>
-        <v>50.685761135253841</v>
+        <v>49.260969559601321</v>
       </c>
       <c r="M12" s="167">
         <f t="shared" si="1"/>
-        <v>2.1119067139689101</v>
+        <v>2.0525403983167219</v>
       </c>
       <c r="N12" s="167"/>
       <c r="O12" s="168" t="s">
         <v>17</v>
       </c>
       <c r="P12" s="167">
-        <v>133197.90767538687</v>
+        <v>137067.88661127014</v>
       </c>
       <c r="Q12" s="167">
         <f t="shared" si="2"/>
-        <v>2219.9651279231143</v>
+        <v>2284.4647768545024</v>
       </c>
       <c r="R12" s="167">
         <f t="shared" si="3"/>
-        <v>92.498546996796435</v>
+        <v>95.186032368937603</v>
       </c>
       <c r="S12" s="167"/>
       <c r="T12" s="168" t="s">
         <v>19</v>
       </c>
       <c r="U12" s="167">
-        <v>37951.072982958824</v>
+        <v>37607.717511190684</v>
       </c>
       <c r="V12" s="167">
         <f t="shared" si="4"/>
-        <v>632.5178830493137</v>
+        <v>626.79529185317801</v>
       </c>
       <c r="W12" s="167">
         <f t="shared" si="5"/>
-        <v>26.354911793721403</v>
+        <v>26.116470493882417</v>
       </c>
       <c r="X12" s="156"/>
       <c r="Y12" s="168"/>
@@ -51660,51 +51642,51 @@
         <v>4</v>
       </c>
       <c r="D13" s="36">
-        <v>0.49688807344275088</v>
+        <v>0.35770545079533922</v>
       </c>
       <c r="J13" s="169" t="s">
         <v>19</v>
       </c>
       <c r="K13" s="167">
-        <v>2014.3482478634555</v>
+        <v>1936.8437710628521</v>
       </c>
       <c r="L13" s="167">
         <f t="shared" si="0"/>
-        <v>33.572470797724257</v>
+        <v>32.2807295177142</v>
       </c>
       <c r="M13" s="167">
         <f t="shared" si="1"/>
-        <v>1.3988529499051774</v>
+        <v>1.345030396571425</v>
       </c>
       <c r="N13" s="167"/>
       <c r="O13" s="168" t="s">
         <v>19</v>
       </c>
       <c r="P13" s="167">
-        <v>63523.192987584647</v>
+        <v>64859.68649390871</v>
       </c>
       <c r="Q13" s="167">
         <f t="shared" si="2"/>
-        <v>1058.7198831264109</v>
+        <v>1080.9947748984785</v>
       </c>
       <c r="R13" s="167">
         <f t="shared" si="3"/>
-        <v>44.113328463600453</v>
+        <v>45.041448954103267</v>
       </c>
       <c r="S13" s="167"/>
       <c r="T13" s="168" t="s">
         <v>18</v>
       </c>
       <c r="U13" s="167">
-        <v>108.36243521062988</v>
+        <v>48.431205452280665</v>
       </c>
       <c r="V13" s="167">
         <f t="shared" si="4"/>
-        <v>1.8060405868438314</v>
+        <v>0.80718675753801106</v>
       </c>
       <c r="W13" s="167">
         <f t="shared" si="5"/>
-        <v>7.5251691118492975E-2</v>
+        <v>3.3632781564083794E-2</v>
       </c>
       <c r="X13" s="156"/>
       <c r="Y13" s="168"/>
@@ -51718,7 +51700,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="36">
-        <v>0.2361447564603604</v>
+        <v>0.1612547245071593</v>
       </c>
       <c r="J14" s="169" t="s">
         <v>18</v>
@@ -51739,40 +51721,66 @@
         <v>18</v>
       </c>
       <c r="P14" s="167">
-        <v>52820.894998603035</v>
+        <v>54772.027248051403</v>
       </c>
       <c r="Q14" s="167">
         <f t="shared" si="2"/>
-        <v>880.34824997671728</v>
+        <v>912.8671208008567</v>
       </c>
       <c r="R14" s="167">
         <f t="shared" si="3"/>
-        <v>36.68117708236322</v>
+        <v>38.036130033369027</v>
       </c>
       <c r="S14" s="167"/>
       <c r="T14" s="168" t="s">
         <v>258</v>
       </c>
       <c r="U14" s="156">
-        <v>5765</v>
+        <v>5718</v>
       </c>
       <c r="V14" s="167"/>
       <c r="W14" s="167"/>
       <c r="X14" s="156"/>
       <c r="Y14" s="168"/>
-      <c r="Z14" s="167"/>
-      <c r="AA14" s="167"/>
-      <c r="AB14" s="167"/>
-      <c r="AC14" s="167"/>
-      <c r="AD14" s="167"/>
-      <c r="AE14" s="167"/>
-      <c r="AF14" s="167"/>
-      <c r="AG14" s="167"/>
-      <c r="AH14" s="167"/>
-      <c r="AI14" s="167"/>
-      <c r="AJ14" s="167"/>
-      <c r="AK14" s="167"/>
-      <c r="AL14" s="185"/>
+      <c r="Z14" s="167">
+        <v>13564.899767855928</v>
+      </c>
+      <c r="AA14" s="167">
+        <v>48451.581006017281</v>
+      </c>
+      <c r="AB14" s="167">
+        <v>11333.492946806178</v>
+      </c>
+      <c r="AC14" s="167">
+        <v>16076.594692398337</v>
+      </c>
+      <c r="AD14" s="167">
+        <v>31271.092095995129</v>
+      </c>
+      <c r="AE14" s="167">
+        <v>13308.28501167484</v>
+      </c>
+      <c r="AF14" s="167">
+        <v>30901.856443803863</v>
+      </c>
+      <c r="AG14" s="167">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="167">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="167">
+        <v>19935.449197617028</v>
+      </c>
+      <c r="AJ14" s="167">
+        <v>18774.361893287652</v>
+      </c>
+      <c r="AK14" s="167">
+        <v>38710.379474175614</v>
+      </c>
+      <c r="AL14" s="185">
+        <v>2186.2857142857142</v>
+      </c>
       <c r="AW14" s="180"/>
     </row>
     <row r="15" spans="1:51" x14ac:dyDescent="0.3">
@@ -51786,7 +51794,7 @@
         <v>258</v>
       </c>
       <c r="K15" s="156">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="L15" s="156"/>
       <c r="M15" s="156"/>
@@ -51795,7 +51803,7 @@
         <v>258</v>
       </c>
       <c r="P15" s="156">
-        <v>14268</v>
+        <v>14153</v>
       </c>
       <c r="Q15" s="156"/>
       <c r="R15" s="156"/>
@@ -51806,19 +51814,45 @@
       <c r="W15" s="156"/>
       <c r="X15" s="156"/>
       <c r="Y15" s="169"/>
-      <c r="Z15" s="167"/>
-      <c r="AA15" s="167"/>
-      <c r="AB15" s="167"/>
-      <c r="AC15" s="167"/>
-      <c r="AD15" s="167"/>
-      <c r="AE15" s="167"/>
-      <c r="AF15" s="167"/>
-      <c r="AG15" s="167"/>
-      <c r="AH15" s="167"/>
-      <c r="AI15" s="167"/>
-      <c r="AJ15" s="167"/>
-      <c r="AK15" s="167"/>
-      <c r="AL15" s="167"/>
+      <c r="Z15" s="167">
+        <v>27596.432957786019</v>
+      </c>
+      <c r="AA15" s="167">
+        <v>68740.152468240689</v>
+      </c>
+      <c r="AB15" s="167">
+        <v>16605.119889451977</v>
+      </c>
+      <c r="AC15" s="167">
+        <v>19865.797401599113</v>
+      </c>
+      <c r="AD15" s="167">
+        <v>60375.441401554308</v>
+      </c>
+      <c r="AE15" s="167">
+        <v>21317.631801080308</v>
+      </c>
+      <c r="AF15" s="167">
+        <v>45094.317425706082</v>
+      </c>
+      <c r="AG15" s="167">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="167">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="167">
+        <v>34823.015038285332</v>
+      </c>
+      <c r="AJ15" s="167">
+        <v>62116.485974991236</v>
+      </c>
+      <c r="AK15" s="167">
+        <v>168646.71305802467</v>
+      </c>
+      <c r="AL15" s="185">
+        <v>2717.7142857142858</v>
+      </c>
       <c r="AW15" s="180"/>
     </row>
     <row r="16" spans="1:51" x14ac:dyDescent="0.3">
@@ -51826,7 +51860,7 @@
         <v>70</v>
       </c>
       <c r="D16" s="36">
-        <v>46.058988118153181</v>
+        <v>31.388154888086948</v>
       </c>
       <c r="J16" s="156"/>
       <c r="K16" s="156"/>
@@ -51848,7 +51882,7 @@
       <c r="AA16" s="156"/>
       <c r="AB16" s="156"/>
     </row>
-    <row r="17" spans="3:38" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:28" x14ac:dyDescent="0.3">
       <c r="C17" s="43" t="s">
         <v>71</v>
       </c>
@@ -51858,43 +51892,43 @@
       <c r="J17" s="156"/>
       <c r="K17" s="167">
         <f>SUM(K2:K14)</f>
-        <v>52375.355633632687</v>
+        <v>51753.336605271987</v>
       </c>
       <c r="L17" s="167">
         <f t="shared" ref="L17" si="14">SUM(L2:L14)</f>
-        <v>872.922593893878</v>
+        <v>862.55561008786651</v>
       </c>
       <c r="M17" s="167">
         <f>SUM(M2:M14)</f>
-        <v>36.37177474557825</v>
+        <v>35.939817086994438</v>
       </c>
       <c r="N17" s="156"/>
       <c r="O17" s="156"/>
       <c r="P17" s="167">
         <f>SUM(P2:P14)</f>
-        <v>892924.5957834</v>
+        <v>913669.66981539899</v>
       </c>
       <c r="Q17" s="167">
         <f t="shared" ref="Q17" si="15">SUM(Q2:Q14)</f>
-        <v>14882.076596390001</v>
+        <v>15227.827830256649</v>
       </c>
       <c r="R17" s="167">
         <f>SUM(R2:R14)</f>
-        <v>620.08652484958327</v>
+        <v>634.49282626069373</v>
       </c>
       <c r="S17" s="156"/>
       <c r="T17" s="156"/>
       <c r="U17" s="167">
         <f t="shared" ref="U17:V17" si="16">SUM(U2:U13)</f>
-        <v>441950.27459222073</v>
+        <v>435962.63704994397</v>
       </c>
       <c r="V17" s="167">
         <f t="shared" si="16"/>
-        <v>7365.8379098703463</v>
+        <v>7266.043950832398</v>
       </c>
       <c r="W17" s="167">
         <f>SUM(W2:W13)</f>
-        <v>306.90991291126443</v>
+        <v>302.75183128468331</v>
       </c>
       <c r="X17" s="156"/>
       <c r="Y17" s="156"/>
@@ -51902,74 +51936,64 @@
       <c r="AA17" s="167"/>
       <c r="AB17" s="167"/>
     </row>
-    <row r="18" spans="3:38" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:28" x14ac:dyDescent="0.3">
       <c r="C18" s="21" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="36">
-        <v>7.7722908934646312E-2</v>
+        <v>6.0705166870574791E-2</v>
       </c>
       <c r="K18" s="156">
         <f t="shared" ref="K18:L18" si="17">K17/$K$15</f>
-        <v>150.5038954989445</v>
+        <v>150.88436328067635</v>
       </c>
       <c r="L18" s="156">
         <f t="shared" si="17"/>
-        <v>2.5083982583157414</v>
+        <v>2.5147393880112725</v>
       </c>
       <c r="M18" s="156">
         <f>M17/$K$15</f>
-        <v>0.10451659409648922</v>
+        <v>0.10478080783380303</v>
       </c>
       <c r="N18" s="156"/>
       <c r="O18" s="156"/>
       <c r="P18" s="156">
         <f t="shared" ref="P18:Q18" si="18">P17/$P$15</f>
-        <v>62.582323786333056</v>
+        <v>64.556607773291816</v>
       </c>
       <c r="Q18" s="156">
         <f t="shared" si="18"/>
-        <v>1.0430387297722177</v>
+        <v>1.0759434628881968</v>
       </c>
       <c r="R18" s="156">
         <f>R17/$P$15</f>
-        <v>4.3459947073842396E-2</v>
+        <v>4.4830977620341536E-2</v>
       </c>
       <c r="S18" s="156"/>
       <c r="T18" s="156"/>
       <c r="U18" s="156">
         <f t="shared" ref="U18:V18" si="19">U17/$U$14</f>
-        <v>76.660932279656677</v>
+        <v>76.243902946824761</v>
       </c>
       <c r="V18" s="156">
         <f t="shared" si="19"/>
-        <v>1.2776822046609446</v>
+        <v>1.2707317157804123</v>
       </c>
       <c r="W18" s="156">
         <f>W17/$U$14</f>
-        <v>5.3236758527539361E-2</v>
+        <v>5.2947154824183856E-2</v>
       </c>
       <c r="Y18" s="156"/>
-      <c r="Z18" s="167"/>
-      <c r="AA18" s="167"/>
-      <c r="AB18" s="167"/>
-      <c r="AC18" s="167"/>
-      <c r="AD18" s="167"/>
-      <c r="AE18" s="167"/>
-      <c r="AF18" s="167"/>
-      <c r="AG18" s="167"/>
-      <c r="AH18" s="167"/>
-      <c r="AI18" s="167"/>
-      <c r="AJ18" s="167"/>
-      <c r="AK18" s="167"/>
-      <c r="AL18" s="167"/>
-    </row>
-    <row r="19" spans="3:38" x14ac:dyDescent="0.3">
+      <c r="Z18" s="156"/>
+      <c r="AA18" s="156"/>
+      <c r="AB18" s="156"/>
+    </row>
+    <row r="19" spans="3:28" x14ac:dyDescent="0.3">
       <c r="C19" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="36">
-        <v>1.6880045300195774E-2</v>
+        <v>1.5459872122206489E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>